<commit_message>
Ready, Error Tasks update
</commit_message>
<xml_diff>
--- a/NEW_robotarmDevelopment_freeRTOS/STM32_PINOUT.xlsx
+++ b/NEW_robotarmDevelopment_freeRTOS/STM32_PINOUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\antal\Documents\STM32\stm32_test_npc\teszt_os\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4806E834-368D-4321-A3F6-A3C3E7D95FD0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B196C0-361B-40C4-B564-096210CFCFD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{917D9E95-D2B8-4B0C-81C1-BE9192EB0E20}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="194">
   <si>
     <t>PA0</t>
   </si>
@@ -489,9 +489,6 @@
     <t>TIM1</t>
   </si>
   <si>
-    <t>COM - MotorR1</t>
-  </si>
-  <si>
     <t>TIM1_CH1</t>
   </si>
   <si>
@@ -607,6 +604,15 @@
   </si>
   <si>
     <t>Button_EMERGENCY</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -760,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -791,6 +797,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1106,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4580C441-249E-47E4-9716-9AAA47CD372B}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24:T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,66 +1124,78 @@
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" customWidth="1"/>
+    <col min="21" max="21" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.85546875" customWidth="1"/>
+    <col min="25" max="25" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" customWidth="1"/>
+    <col min="29" max="29" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>132</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="30"/>
+      <c r="F1" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="30"/>
+      <c r="J1" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>133</v>
-      </c>
+      <c r="L1" s="30"/>
       <c r="N1" s="12" t="s">
         <v>132</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" s="26" t="s">
-        <v>183</v>
+      <c r="P1" s="30"/>
+      <c r="R1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="T1" s="30"/>
+      <c r="V1" s="26" t="s">
+        <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -1186,32 +1205,36 @@
       <c r="C2" t="s">
         <v>131</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="F2" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="G2" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28"/>
+      <c r="J2" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="L2" s="25"/>
+      <c r="N2" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="L2" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="P2" s="23"/>
+      <c r="R2" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>150</v>
       </c>
+      <c r="T2" s="13"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -1221,26 +1244,28 @@
       <c r="C3" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="19"/>
+      <c r="J3" t="s">
         <v>144</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>145</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="N3" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="L3" s="25" t="s">
-        <v>182</v>
-      </c>
+      <c r="O3" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="P3" s="25"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>151</v>
       </c>
@@ -1250,26 +1275,29 @@
       <c r="C4" t="s">
         <v>137</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="21"/>
+      <c r="J4" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="L4" s="16" t="s">
+      <c r="K4" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="L4" s="25"/>
+      <c r="N4" s="16" t="s">
         <v>162</v>
       </c>
+      <c r="O4" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="P4" s="16"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12" t="s">
         <v>134</v>
@@ -1278,26 +1306,22 @@
         <v>135</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="K6" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>135</v>
-      </c>
+      <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="12" t="s">
         <v>134</v>
@@ -1306,568 +1330,626 @@
         <v>135</v>
       </c>
       <c r="P6" s="12"/>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="S6" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12" t="s">
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="U6" s="12" t="s">
+      <c r="W6" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12" t="s">
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="X6" s="12" t="s">
+      <c r="AA6" s="12" t="s">
         <v>135</v>
       </c>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE6" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="Y7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="T7" s="3" t="str">
+      <c r="Z7" s="3" t="str">
         <f>_xlfn.CONCAT("ButtonPos - ", B2)</f>
         <v>ButtonPos - MotorR1</v>
       </c>
-      <c r="U7" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="V7" s="2" t="s">
+      <c r="AA7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="U8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="Y8" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="T8" s="3" t="str">
+      <c r="Z8" s="3" t="str">
         <f>_xlfn.CONCAT("ButtonNeg - ", B2)</f>
         <v>ButtonNeg - MotorR1</v>
       </c>
-      <c r="U8" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="V8" s="2" t="s">
+      <c r="AA8" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D9" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="U9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="Y9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="T9" s="3" t="str">
+      <c r="Z9" s="3" t="str">
         <f>_xlfn.CONCAT("LSPos - ", B2)</f>
         <v>LSPos - MotorR1</v>
       </c>
-      <c r="U9" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="V9" s="2" t="s">
+      <c r="AA9" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="D10" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="U10" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="Q10" s="11" t="str">
+      <c r="V10" s="11" t="str">
         <f>_xlfn.CONCAT("ButtonPos - ", B4)</f>
         <v>ButtonPos - MotorPVertical</v>
       </c>
-      <c r="R10" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="S10" s="4" t="s">
+      <c r="W10" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="T10" s="3" t="str">
+      <c r="Z10" s="3" t="str">
         <f>_xlfn.CONCAT("LSNeg - ", B2)</f>
         <v>LSNeg - MotorR1</v>
       </c>
-      <c r="U10" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="V10" s="2" t="s">
+      <c r="AA10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="U11" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Q11" s="11" t="str">
+      <c r="V11" s="11" t="str">
         <f>_xlfn.CONCAT("ButtonNeg - ", B4)</f>
         <v>ButtonNeg - MotorPVertical</v>
       </c>
-      <c r="R11" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="S11" s="6" t="s">
+      <c r="W11" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="T11" s="5" t="str">
+      <c r="Z11" s="5" t="str">
         <f>_xlfn.CONCAT("LSPos - ", B3)</f>
         <v>LSPos - MotorPHorizontal</v>
       </c>
-      <c r="U11" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="V11" s="2" t="s">
+      <c r="AA11" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C12" s="23"/>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="23"/>
+      <c r="E12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="U12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S12" s="6" t="s">
+      <c r="Y12" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="T12" s="5" t="str">
+      <c r="Z12" s="5" t="str">
         <f>_xlfn.CONCAT("LSNeg - ", B3)</f>
         <v>LSNeg - MotorPHorizontal</v>
       </c>
-      <c r="U12" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="V12" s="2" t="s">
+      <c r="AA12" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="U13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="Y13" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="T13" s="7" t="str">
+      <c r="Z13" s="7" t="str">
         <f>_xlfn.CONCAT("LSPos - ", B4)</f>
         <v>LSPos - MotorPVertical</v>
       </c>
-      <c r="U13" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="V13" s="2" t="s">
+      <c r="AA13" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" s="23"/>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="23"/>
+      <c r="E14" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="14" t="s">
+      <c r="F14" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="J14" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K14" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="L14" s="13"/>
+      <c r="M14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="Q14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="U14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S14" s="8" t="s">
+      <c r="Y14" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="T14" s="7" t="str">
+      <c r="Z14" s="7" t="str">
         <f>_xlfn.CONCAT("LSNeg - ", B4)</f>
         <v>LSNeg - MotorPVertical</v>
       </c>
-      <c r="U14" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="V14" s="2" t="s">
+      <c r="AA14" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="I15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="5" t="str">
+      <c r="J15" s="5" t="str">
         <f>_xlfn.CONCAT("DIR - ",B3)</f>
         <v>DIR - MotorPHorizontal</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="U15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S15" s="27" t="s">
+      <c r="Y15" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="T15" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="U15" s="25"/>
-      <c r="V15" s="2" t="s">
+      <c r="Z15" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA15" s="25"/>
+      <c r="AB15" s="25"/>
+      <c r="AC15" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="D16" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="Q16" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="R16" s="3" t="str">
+        <f>_xlfn.CONCAT("STEP - ", B2)</f>
+        <v>STEP - MotorR1</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="U16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S16" s="17" t="s">
+      <c r="Y16" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="T16" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="U16" s="16" t="s">
+      <c r="Z16" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="V16" s="2" t="s">
+      <c r="AA16" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="D17" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="Q17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="N17" s="3" t="str">
-        <f>_xlfn.CONCAT("STEP - ", B2)</f>
-        <v>STEP - MotorR1</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="P17" s="2" t="s">
+      <c r="U17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S17" s="17" t="s">
+      <c r="Y17" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="T17" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="U17" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="V17" s="2" t="s">
+      <c r="Z17" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA17" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB17" s="16"/>
+      <c r="AC17" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="5" t="str">
+      <c r="J18" s="5" t="str">
         <f>_xlfn.CONCAT("ENABLE - ",B3)</f>
         <v>ENABLE - MotorPHorizontal</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="Q18" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="N18" s="5" t="str">
+      <c r="R18" s="5" t="str">
         <f xml:space="preserve"> _xlfn.CONCAT("STEP - ",B3)</f>
         <v>STEP - MotorPHorizontal</v>
       </c>
-      <c r="O18" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="P18" s="2" t="s">
+      <c r="S18" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="U18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="S18" s="29" t="s">
+      <c r="Y18" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="T18" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="U18" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="V18" s="2" t="s">
+      <c r="Z18" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA18" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="5" t="str">
+      <c r="J19" s="5" t="str">
         <f>_xlfn.CONCAT("COM - ", B3)</f>
         <v>COM - MotorPHorizontal</v>
       </c>
-      <c r="I19" s="5">
+      <c r="K19" s="5">
         <v>0</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="L19" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="M19" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="K19" s="16" t="s">
+      <c r="N19" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="O19" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="L19" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="M19" s="4" t="s">
+      <c r="P19" s="18"/>
+      <c r="Q19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="N19" s="3" t="str">
+      <c r="R19" s="3" t="str">
         <f>_xlfn.CONCAT("DIR - ",B2)</f>
         <v>DIR - MotorR1</v>
       </c>
-      <c r="O19" s="3"/>
-      <c r="P19" s="2" t="s">
+      <c r="S19" s="3"/>
+      <c r="T19" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="U19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="Y19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="V19" s="2" t="s">
+      <c r="AC19" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
@@ -1876,49 +1958,57 @@
         <v>ButtonPos - MotorPHorizontal</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D20" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="I20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="7" t="str">
+      <c r="J20" s="7" t="str">
         <f>_xlfn.CONCAT("DIR - ",B4)</f>
         <v>DIR - MotorPVertical</v>
       </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="17" t="s">
+      <c r="K20" s="7"/>
+      <c r="L20" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="M20" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="K20" s="16" t="s">
+      <c r="N20" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="O20" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="L20" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="M20" s="8" t="s">
+      <c r="P20" s="18"/>
+      <c r="Q20" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N20" s="7" t="str">
+      <c r="R20" s="7" t="str">
         <f>_xlfn.CONCAT("STEP - ", B4)</f>
         <v>STEP - MotorPVertical</v>
       </c>
-      <c r="O20" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="P20" s="2" t="s">
+      <c r="S20" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="U20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="Y20" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="V20" s="2" t="s">
+      <c r="AC20" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -1927,99 +2017,123 @@
         <v>ButtonNeg - MotorPHorizontal</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D21" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="I21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="7" t="str">
+      <c r="J21" s="7" t="str">
         <f>_xlfn.CONCAT("ENABLE - ",B4)</f>
         <v>ENABLE - MotorPVertical</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="17" t="s">
+      <c r="K21" s="7"/>
+      <c r="L21" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="M21" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="N21" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="O21" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="L21" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="M21" s="4" t="s">
+      <c r="P21" s="18"/>
+      <c r="Q21" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="N21" s="3" t="str">
+      <c r="R21" s="3" t="str">
         <f>_xlfn.CONCAT("COM - ", B2)</f>
         <v>COM - MotorR1</v>
       </c>
-      <c r="O21" s="3">
+      <c r="S21" s="3">
         <v>0</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="T21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="U21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="Y21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="AC21" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="9" t="str">
+      <c r="J22" s="9" t="str">
         <f>_xlfn.CONCAT("COM - ", B4)</f>
         <v>COM - MotorPVertical</v>
       </c>
-      <c r="I22" s="9">
+      <c r="K22" s="9">
         <v>0</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="L22" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="4" t="s">
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N22" s="3" t="str">
+      <c r="R22" s="3" t="str">
         <f>_xlfn.CONCAT("ENABLE - ",B2)</f>
         <v>ENABLE - MotorR1</v>
       </c>
-      <c r="O22" s="3">
+      <c r="S22" s="3">
         <v>0</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="T22" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="U22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="2" t="s">
-        <v>127</v>
-      </c>
+      <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
+      <c r="Y22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="T25" t="s">
+        <v>192</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>